<commit_message>
Proyecto listo para despliegue
</commit_message>
<xml_diff>
--- a/data/candidatos.xlsx
+++ b/data/candidatos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2868,6 +2868,588 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>juan diego</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ramirez rendon</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ramirezrendonjuandiego54@gmail.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+573116347492</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2007-08-21</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>['Python', 'JavaScript', 'HTML', 'CSS', 'Flask']</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>10</v>
+      </c>
+      <c r="J26" t="n">
+        <v>100</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>itagui</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>7</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>['Comunicación', 'Adaptabilidad', 'Creatividad', 'Empatía', 'Escucha activa']</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>['Inglés', 'Español']</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>backend</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>['Autonomía']</t>
+        </is>
+      </c>
+      <c r="T26" t="n">
+        <v>345</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>lider_equipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ospina baena</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>miguelospinabaena@gmail.com</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>+573213983128</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2008-02-18</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>['JavaScript', 'Java', 'HTML', 'CSS']</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>8</v>
+      </c>
+      <c r="J27" t="n">
+        <v>85</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>1623508</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>3</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>['Comunicación', 'Adaptabilidad', 'Empatía', 'Gestión del tiempo']</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>['Inglés', 'Español', 'Francés']</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>backend</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>['Organización', 'Empatía', 'Autonomía', 'Comunicación', 'Curiosidad', 'Perseverancia', 'Compromiso']</t>
+        </is>
+      </c>
+      <c r="T27" t="n">
+        <v>450</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>lider_equipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ospina baena</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>miguelospinabaena@gmail.com</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>+573213983128</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2008-02-18</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>['JavaScript', 'Java', 'HTML', 'CSS']</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>8</v>
+      </c>
+      <c r="J28" t="n">
+        <v>85</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>1623508</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>3</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>['Comunicación', 'Adaptabilidad', 'Empatía', 'Gestión del tiempo']</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>['Inglés', 'Español', 'Francés']</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>backend</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>['Organización', 'Empatía', 'Autonomía', 'Comunicación', 'Curiosidad', 'Perseverancia', 'Compromiso']</t>
+        </is>
+      </c>
+      <c r="T28" t="n">
+        <v>450</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>lider_equipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ospina baena</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>miguelospinabaena@gmail.com</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>+573213983128</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2008-02-18</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>['JavaScript', 'Java', 'HTML', 'CSS']</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>8</v>
+      </c>
+      <c r="J29" t="n">
+        <v>85</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>1623508</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>3</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>['Comunicación', 'Adaptabilidad', 'Empatía', 'Gestión del tiempo']</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>['Inglés', 'Español', 'Francés']</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>backend</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>['Organización', 'Empatía', 'Autonomía', 'Comunicación', 'Curiosidad', 'Perseverancia', 'Compromiso']</t>
+        </is>
+      </c>
+      <c r="T29" t="n">
+        <v>450</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>lider_equipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>miguel</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ospina baena</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>miguelospinabaena@gmail.com</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>+573213983128</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2008-02-18</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>['JavaScript', 'Java', 'HTML', 'CSS']</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>8</v>
+      </c>
+      <c r="J30" t="n">
+        <v>85</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>1623508</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>3</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>['Comunicación', 'Adaptabilidad', 'Empatía', 'Gestión del tiempo']</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>['Inglés', 'Español', 'Francés']</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>backend</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>['Organización', 'Empatía', 'Autonomía', 'Comunicación', 'Curiosidad', 'Perseverancia', 'Compromiso']</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>450</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>lider_equipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>juan diego</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ramirez rendon</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ramirezrendonjuandiego5@gmail.com</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>+573116347491</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2007-08-21</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>['AWS']</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>10</v>
+      </c>
+      <c r="J31" t="n">
+        <v>100</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L31" t="n">
+        <v>1623500</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>itagui</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>7</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>['Comunicación']</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>['Español']</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>frontend</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>['Autonomía']</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>345</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>emprender</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>